<commit_message>
slide báo cáo, cập nhật file báo cáo, file nhật ký, file kế hoạch
</commit_message>
<xml_diff>
--- a/TaiLieu/KeHoach.xlsx
+++ b/TaiLieu/KeHoach.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Ke hoach thuc hien" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>KẾ HOẠCH THỰC HIỆN ĐỒ ÁN</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Châu Thị Bảo Hà</t>
+  </si>
+  <si>
+    <t>- Báo cáo và phản biện.</t>
   </si>
 </sst>
 </file>
@@ -708,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1019,9 @@
         <f t="shared" si="0"/>
         <v>44003</v>
       </c>
-      <c r="D20" s="16"/>
+      <c r="D20" s="16" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>